<commit_message>
Music / Comment / Tag 데이터 삽입
</commit_message>
<xml_diff>
--- a/myhomework17_1/myhomework17.xlsx
+++ b/myhomework17_1/myhomework17.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
   <si>
     <t>title</t>
   </si>
@@ -22,18 +22,12 @@
     <t>album</t>
   </si>
   <si>
-    <t>genre</t>
-  </si>
-  <si>
     <t>released_date</t>
   </si>
   <si>
     <t>description</t>
   </si>
   <si>
-    <t>korean_music</t>
-  </si>
-  <si>
     <t>ASAP</t>
   </si>
   <si>
@@ -41,9 +35,6 @@
   </si>
   <si>
     <t>STAYDOM</t>
-  </si>
-  <si>
-    <t>댄스</t>
   </si>
   <si>
     <t>2021.4.8</t>
@@ -111,9 +102,6 @@
     <t>너없인 안된다</t>
   </si>
   <si>
-    <t>발라드</t>
-  </si>
-  <si>
     <t>Composed, Arranged by 임현식, 이든(EDEN)
 Lyrics by 임현식, 이든(EDEN), 이민혁, 프니엘, 정일훈
 타이틀곡 ‘너 없인 안 된다’는 청량함이 물씬 느껴지는 신스 패턴과 서정적인 어쿠스틱 사운드 위로 멤버 각자의 개성 있는 보이스 톤을 만끽할 수 있는 팝 발라드 장르의 곡으로 그리워하던 그녀를 향한 남자의 절절한 고백을 간절하지만 부드럽게 풀어냈다.</t>
@@ -242,9 +230,6 @@
     <t>OK ORCHESTRA</t>
   </si>
   <si>
-    <t>팝</t>
-  </si>
-  <si>
     <t>2021.03.26</t>
   </si>
   <si>
@@ -264,9 +249,6 @@
     <t>ORION</t>
   </si>
   <si>
-    <t>록/메탈</t>
-  </si>
-  <si>
     <t>2019.06.14</t>
   </si>
   <si>
@@ -280,7 +262,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -290,7 +272,6 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color rgb="FF606060"/>
       <name val="&quot;맑은 고딕&quot;"/>
@@ -321,23 +302,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -572,333 +550,243 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="b">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="1" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="1" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="1" t="b">
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="1" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="2" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="1" t="b">
-        <v>1</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="1" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="1" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="1" t="b">
-        <v>1</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G14" s="2" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="1" t="b">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>